<commit_message>
Made relevant changes and created second stream table
</commit_message>
<xml_diff>
--- a/Equipment Size, Stream Tables, Solutes Info/stream table NABEER.xlsx
+++ b/Equipment Size, Stream Tables, Solutes Info/stream table NABEER.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5817112240c0c948/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Soumya\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA5749A8-311C-45BB-9CA4-A8DF97D0B11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{FA5749A8-311C-45BB-9CA4-A8DF97D0B11B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8FBF34C2-9BE3-40C9-949F-41C18ECA76F3}"/>
   <bookViews>
-    <workbookView xWindow="14250" yWindow="960" windowWidth="14550" windowHeight="14640" xr2:uid="{902E8129-377E-4200-9527-4DDE2ED6D044}"/>
+    <workbookView xWindow="14250" yWindow="960" windowWidth="14550" windowHeight="14640" activeTab="1" xr2:uid="{902E8129-377E-4200-9527-4DDE2ED6D044}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="time = 0" sheetId="1" r:id="rId1"/>
+    <sheet name="time =6167" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="181029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>Ethanol</t>
   </si>
@@ -51,9 +52,6 @@
     <t>split ratio</t>
   </si>
   <si>
-    <t>volume 6+8</t>
-  </si>
-  <si>
     <t>Ethanol permeate rate</t>
   </si>
   <si>
@@ -66,12 +64,6 @@
     <t>membrane 2</t>
   </si>
   <si>
-    <t>membrane area</t>
-  </si>
-  <si>
-    <t>cm2</t>
-  </si>
-  <si>
     <t>basis 1 second</t>
   </si>
   <si>
@@ -109,6 +101,24 @@
   </si>
   <si>
     <t>other</t>
+  </si>
+  <si>
+    <t>volume 4+8</t>
+  </si>
+  <si>
+    <t>Stream</t>
+  </si>
+  <si>
+    <t>obtained from python simulation</t>
+  </si>
+  <si>
+    <t>feed solutes</t>
+  </si>
+  <si>
+    <t>feed ethanol</t>
+  </si>
+  <si>
+    <t>Feed water</t>
   </si>
 </sst>
 </file>
@@ -132,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -145,8 +155,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -154,14 +170,128 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,24 +606,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2679D219-28F4-4F72-B53C-D50F00EC4B94}">
-  <dimension ref="A3:L31"/>
+  <dimension ref="A3:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="64" workbookViewId="0">
-      <selection activeCell="D43" sqref="D43"/>
+    <sheetView zoomScale="51" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" customWidth="1"/>
     <col min="6" max="6" width="20.140625" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" customWidth="1"/>
     <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -504,180 +639,191 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="C6" s="1">
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>3</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="6">
         <v>4</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="6">
         <v>5</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="6">
         <v>6</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="6">
         <v>7</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="6">
         <v>8</v>
       </c>
-      <c r="K6" s="1">
+      <c r="K6" s="6">
         <v>9</v>
       </c>
-      <c r="L6" s="1">
+      <c r="L6" s="7">
         <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="8">
         <v>0</v>
       </c>
-      <c r="D7">
-        <v>3.9460000000000002E-2</v>
-      </c>
-      <c r="E7">
-        <f>C7+D7</f>
-        <v>3.9460000000000002E-2</v>
-      </c>
-      <c r="F7">
-        <f>E7*$H$14</f>
-        <v>1.9730000000000004E-3</v>
-      </c>
-      <c r="G7">
+      <c r="D7" s="9">
+        <f>E7-C7-L7</f>
+        <v>30.060000000000002</v>
+      </c>
+      <c r="E7" s="8">
+        <f>$E$10*$F$40</f>
+        <v>35.514000000000003</v>
+      </c>
+      <c r="F7" s="8">
+        <f>H15</f>
+        <v>14.25</v>
+      </c>
+      <c r="G7" s="8">
         <f>E7-F7</f>
-        <v>3.7486999999999999E-2</v>
-      </c>
-      <c r="H7">
-        <v>0.02</v>
-      </c>
-      <c r="I7">
+        <v>21.264000000000003</v>
+      </c>
+      <c r="H7" s="8">
+        <f>G7*$H$14</f>
+        <v>1.0632000000000001</v>
+      </c>
+      <c r="I7" s="8">
         <f>G7-H7</f>
-        <v>1.7486999999999999E-2</v>
-      </c>
-      <c r="J7">
+        <v>20.200800000000001</v>
+      </c>
+      <c r="J7" s="8">
         <f>H17</f>
-        <v>0.01</v>
-      </c>
-      <c r="K7">
-        <v>4</v>
-      </c>
-      <c r="L7">
-        <f>K7+F7</f>
-        <v>4.0019729999999996</v>
+        <v>15.81</v>
+      </c>
+      <c r="K7" s="8">
+        <f>I7-J7</f>
+        <v>4.3908000000000005</v>
+      </c>
+      <c r="L7" s="10">
+        <f>K7+H7</f>
+        <v>5.4540000000000006</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="11">
         <f>$H$13*997000</f>
-        <v>13.994952573700346</v>
-      </c>
-      <c r="D8">
-        <f>100-D7-D9</f>
-        <v>99.940539999999999</v>
-      </c>
-      <c r="E8">
-        <f>C8+D8</f>
-        <v>113.93549257370034</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ref="F8:F9" si="0">E8*$H$14</f>
-        <v>5.6967746286850174</v>
-      </c>
-      <c r="G8">
+        <v>1342.6029565182259</v>
+      </c>
+      <c r="D8" s="12">
+        <f>E8-C8-L8</f>
+        <v>-525.40695651822625</v>
+      </c>
+      <c r="E8" s="11">
+        <f>E10*F41</f>
+        <v>8665.2732000000015</v>
+      </c>
+      <c r="F8" s="11">
+        <f>H16</f>
+        <v>408.59800000000001</v>
+      </c>
+      <c r="G8" s="11">
         <f>E8-F8</f>
-        <v>108.23871794501532</v>
-      </c>
-      <c r="H8">
-        <v>5</v>
-      </c>
-      <c r="I8">
-        <f>G8-H8</f>
-        <v>103.23871794501532</v>
-      </c>
-      <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8">
-        <v>7</v>
-      </c>
-      <c r="L8">
-        <f t="shared" ref="L8:L9" si="1">K8+F8</f>
-        <v>12.696774628685016</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+        <v>8256.6752000000015</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" ref="H8:H9" si="0">G8*$H$14</f>
+        <v>412.8337600000001</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" ref="I8:I9" si="1">G8-H8</f>
+        <v>7843.8414400000011</v>
+      </c>
+      <c r="J8" s="11">
+        <f>H18</f>
+        <v>408.59800000000001</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" ref="K8:K9" si="2">I8-J8</f>
+        <v>7435.2434400000011</v>
+      </c>
+      <c r="L8" s="13">
+        <f t="shared" ref="L8:L9" si="3">K8+H8</f>
+        <v>7848.0772000000015</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="14">
         <v>0</v>
       </c>
-      <c r="D9" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="E9">
-        <f>C9+D9</f>
-        <v>0.02</v>
-      </c>
-      <c r="F9">
+      <c r="D9" s="15">
+        <f>E9-C9-L9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <f>$E$10*$F$39</f>
+        <v>299.21280000000002</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <f>E9-F9</f>
+        <v>299.21280000000002</v>
+      </c>
+      <c r="H9" s="14">
         <f t="shared" si="0"/>
-        <v>1E-3</v>
-      </c>
-      <c r="G9">
-        <f>E9-F9</f>
-        <v>1.9E-2</v>
-      </c>
-      <c r="H9">
+        <v>14.960640000000001</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="1"/>
+        <v>284.25216</v>
+      </c>
+      <c r="J9" s="14">
         <v>0</v>
       </c>
-      <c r="I9">
-        <f>G9-H9</f>
-        <v>1.9E-2</v>
-      </c>
-      <c r="J9">
-        <v>0</v>
-      </c>
-      <c r="K9">
-        <f t="shared" ref="K8:K9" si="2">I9-J9</f>
-        <v>1.9E-2</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
+      <c r="K9" s="14">
+        <f t="shared" si="2"/>
+        <v>284.25216</v>
+      </c>
+      <c r="L9" s="16">
+        <f t="shared" si="3"/>
+        <v>299.21280000000002</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>17</v>
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>900</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G13" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="H13">
         <f>F26+G26</f>
-        <v>1.4037063764995332E-5</v>
+        <v>1.3466428851737471E-3</v>
       </c>
       <c r="I13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -690,66 +836,68 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H15" s="2">
-        <v>2.0000000000000001E-4</v>
+        <v>14.25</v>
       </c>
       <c r="I15" t="s">
-        <v>18</v>
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H16" s="2">
-        <v>2E-3</v>
+        <v>408.59800000000001</v>
       </c>
       <c r="I16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H17" s="2">
-        <v>0.01</v>
+        <v>15.81</v>
       </c>
       <c r="I17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="G18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H18" s="2">
-        <v>2.0000000000000001E-4</v>
+        <v>408.59800000000001</v>
       </c>
       <c r="I18" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="G20" t="s">
-        <v>11</v>
-      </c>
-      <c r="H20" s="2"/>
-      <c r="I20" t="s">
-        <v>12</v>
-      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
       <c r="F22">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G22">
         <v>8</v>
@@ -757,39 +905,39 @@
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="E23" t="s">
         <v>0</v>
       </c>
       <c r="F23">
-        <f>H7/802000</f>
-        <v>2.4937655860349126E-8</v>
+        <f>F7/802000</f>
+        <v>1.7768079800498752E-5</v>
       </c>
       <c r="G23">
         <f>J8/802400</f>
-        <v>4.9850448654037884E-6</v>
+        <v>5.0921984047856434E-4</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
         <v>2</v>
       </c>
       <c r="F24">
-        <f>H8/997000</f>
-        <v>5.0150451354062186E-6</v>
+        <f>F8/997000</f>
+        <v>4.0982748244734204E-4</v>
       </c>
       <c r="G24">
         <f>J8/997000</f>
-        <v>4.0120361083249752E-6</v>
+        <v>4.0982748244734204E-4</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E25" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F25">
         <v>0</v>
@@ -800,43 +948,509 @@
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E26" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F26">
         <f>SUM(F23:F25)</f>
-        <v>5.039982791266568E-6</v>
+        <v>4.275955622478408E-4</v>
       </c>
       <c r="G26">
         <f>SUM(G23:G25)</f>
-        <v>8.9970809737287636E-6</v>
+        <v>9.1904732292590638E-4</v>
       </c>
       <c r="H26" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="F30">
         <v>802.4</v>
       </c>
       <c r="G30" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H30" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="E31" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F31">
         <v>997</v>
       </c>
       <c r="G31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39">
+        <f>12.4672*10000/375</f>
+        <v>332.45866666666666</v>
+      </c>
+      <c r="F39">
+        <f t="shared" ref="F39" si="4">E39/1000</f>
+        <v>0.33245866666666668</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40">
+        <f>0.03946*1000</f>
+        <v>39.46</v>
+      </c>
+      <c r="F40">
+        <f>E40/1000</f>
+        <v>3.9460000000000002E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41">
+        <f>10000-E40-E39</f>
+        <v>9628.0813333333335</v>
+      </c>
+      <c r="F41">
+        <f t="shared" ref="F41" si="5">E41/1000</f>
+        <v>9.6280813333333342</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B18B83C8-1203-428B-AC55-6DD7D62FDB4F}">
+  <dimension ref="A3:L41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
+      <selection activeCell="G36" sqref="G36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="20.140625" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" customWidth="1"/>
+    <col min="6" max="6" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="13.42578125" customWidth="1"/>
+    <col min="11" max="11" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="5">
+        <v>2</v>
+      </c>
+      <c r="E6" s="6">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6">
+        <v>5</v>
+      </c>
+      <c r="H6" s="6">
+        <v>6</v>
+      </c>
+      <c r="I6" s="6">
+        <v>7</v>
+      </c>
+      <c r="J6" s="6">
+        <v>8</v>
+      </c>
+      <c r="K6" s="6">
+        <v>9</v>
+      </c>
+      <c r="L6" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B7" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9">
+        <f>E7-C7-L7</f>
+        <v>3.0243856999999998</v>
+      </c>
+      <c r="E7" s="8">
+        <f>$E$10*$F$40</f>
+        <v>3.5549729999999999</v>
+      </c>
+      <c r="F7" s="8">
+        <f>H15</f>
+        <v>1.4514857000000001</v>
+      </c>
+      <c r="G7" s="8">
+        <f>E7-F7</f>
+        <v>2.1034872999999998</v>
+      </c>
+      <c r="H7" s="8">
+        <f>G7*$H$14</f>
+        <v>0.10517436499999999</v>
+      </c>
+      <c r="I7" s="8">
+        <f>G7-H7</f>
+        <v>1.998312935</v>
+      </c>
+      <c r="J7" s="8">
+        <f>H17</f>
+        <v>1.5729</v>
+      </c>
+      <c r="K7" s="8">
+        <f>I7-J7</f>
+        <v>0.42541293499999999</v>
+      </c>
+      <c r="L7" s="10">
+        <f>K7+H7</f>
+        <v>0.53058729999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B8" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="11">
+        <f>$H$13*997000</f>
+        <v>1326.6925840031388</v>
+      </c>
+      <c r="D8" s="12">
+        <f>E8-C8-L8</f>
+        <v>-509.49658400313876</v>
+      </c>
+      <c r="E8" s="11">
+        <f>E10*F41</f>
+        <v>866.56502699999999</v>
+      </c>
+      <c r="F8" s="11">
+        <f>H16</f>
+        <v>408.59800000000001</v>
+      </c>
+      <c r="G8" s="11">
+        <f>E8-F8</f>
+        <v>457.96702699999997</v>
+      </c>
+      <c r="H8" s="11">
+        <f t="shared" ref="H8:H9" si="0">G8*$H$14</f>
+        <v>22.898351349999999</v>
+      </c>
+      <c r="I8" s="11">
+        <f t="shared" ref="I8:I9" si="1">G8-H8</f>
+        <v>435.06867564999999</v>
+      </c>
+      <c r="J8" s="11">
+        <f>H18</f>
+        <v>408.59800000000001</v>
+      </c>
+      <c r="K8" s="11">
+        <f t="shared" ref="K8:K9" si="2">I8-J8</f>
+        <v>26.470675649999976</v>
+      </c>
+      <c r="L8" s="13">
+        <f t="shared" ref="L8:L9" si="3">K8+H8</f>
+        <v>49.369026999999974</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="14">
+        <v>0</v>
+      </c>
+      <c r="D9" s="15">
+        <f>E9-C9-L9</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="14">
+        <f>$E$10*$F$39</f>
+        <v>29.88</v>
+      </c>
+      <c r="F9" s="14">
+        <v>0</v>
+      </c>
+      <c r="G9" s="14">
+        <f>E9-F9</f>
+        <v>29.88</v>
+      </c>
+      <c r="H9" s="14">
+        <f t="shared" si="0"/>
+        <v>1.494</v>
+      </c>
+      <c r="I9" s="14">
+        <f t="shared" si="1"/>
+        <v>28.385999999999999</v>
+      </c>
+      <c r="J9" s="14">
+        <v>0</v>
+      </c>
+      <c r="K9" s="14">
+        <f t="shared" si="2"/>
+        <v>28.385999999999999</v>
+      </c>
+      <c r="L9" s="16">
+        <f t="shared" si="3"/>
+        <v>29.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <f>F26+G26</f>
+        <v>1.3306846379168894E-3</v>
+      </c>
+      <c r="I13" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H14">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" t="s">
+        <v>6</v>
+      </c>
+      <c r="H15" s="2">
+        <v>1.4514857000000001</v>
+      </c>
+      <c r="I15" t="s">
+        <v>15</v>
+      </c>
+      <c r="J15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2">
+        <v>408.59800000000001</v>
+      </c>
+      <c r="I16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="F17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="H17" s="2">
+        <v>1.5729</v>
+      </c>
+      <c r="I17" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>7</v>
+      </c>
+      <c r="H18" s="2">
+        <v>408.59800000000001</v>
+      </c>
+      <c r="I18" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+      <c r="G22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <f>F7/802000</f>
+        <v>1.809832543640898E-6</v>
+      </c>
+      <c r="G23">
+        <f>J8/802400</f>
+        <v>5.0921984047856434E-4</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
         <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <f>F8/997000</f>
+        <v>4.0982748244734204E-4</v>
+      </c>
+      <c r="G24">
+        <f>J8/997000</f>
+        <v>4.0982748244734204E-4</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26">
+        <f>SUM(F23:F25)</f>
+        <v>4.1163731499098291E-4</v>
+      </c>
+      <c r="G26">
+        <f>SUM(G23:G25)</f>
+        <v>9.1904732292590638E-4</v>
+      </c>
+      <c r="H26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>17</v>
+      </c>
+      <c r="F30">
+        <v>802.4</v>
+      </c>
+      <c r="G30" t="s">
+        <v>18</v>
+      </c>
+      <c r="H30" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>997</v>
+      </c>
+      <c r="G31" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E39">
+        <v>3.32</v>
+      </c>
+      <c r="F39">
+        <f>E39/100</f>
+        <v>3.32E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D40" t="s">
+        <v>27</v>
+      </c>
+      <c r="E40">
+        <f>0.00394997*100</f>
+        <v>0.39499699999999999</v>
+      </c>
+      <c r="F40">
+        <f>E40/100</f>
+        <v>3.9499699999999997E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="4:6" x14ac:dyDescent="0.25">
+      <c r="D41" t="s">
+        <v>28</v>
+      </c>
+      <c r="E41">
+        <f>100-E40-E39</f>
+        <v>96.285003000000003</v>
+      </c>
+      <c r="F41">
+        <f>E41/100</f>
+        <v>0.96285003000000002</v>
       </c>
     </row>
   </sheetData>
@@ -1031,18 +1645,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1065,14 +1679,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5999BF9-8FA3-461F-AF70-A5CBD70059D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE420947-E82C-44D4-9586-9CD1CA91B220}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="dcd3136c-638f-4341-9ade-e46389e4a53d"/>
@@ -1087,4 +1693,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5999BF9-8FA3-461F-AF70-A5CBD70059D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>